<commit_message>
back to render point clouds with same number of points
</commit_message>
<xml_diff>
--- a/process_final.xlsx
+++ b/process_final.xlsx
@@ -8,6 +8,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -62,7 +63,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F90"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="true"/>
@@ -75,19 +76,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0">
-        <v>504</v>
+        <v>360</v>
       </c>
       <c r="B1" s="0">
-        <v>60.415994349237486</v>
+        <v>40.717526290664516</v>
       </c>
       <c r="C1" s="0">
-        <v>60.415229867972855</v>
+        <v>40.804411526206337</v>
       </c>
       <c r="D1" s="0">
-        <v>2.9032300676354215</v>
+        <v>2.8304454991108989</v>
       </c>
       <c r="E1" s="0">
-        <v>2.4365301257266767e-16</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="F1" s="0">
         <v>3.0000000000000004</v>
@@ -95,19 +96,19 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>320</v>
+        <v>360</v>
       </c>
       <c r="B2" s="0">
-        <v>37.603890819287187</v>
+        <v>40.717526290664516</v>
       </c>
       <c r="C2" s="0">
-        <v>37.603191353926334</v>
+        <v>40.804411526206337</v>
       </c>
       <c r="D2" s="0">
-        <v>2.8478822362349114</v>
+        <v>2.8304454991108989</v>
       </c>
       <c r="E2" s="0">
-        <v>8.1224339918031972e-16</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="F2" s="0">
         <v>3.0000000000000004</v>
@@ -115,19 +116,19 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>436</v>
+        <v>336</v>
       </c>
       <c r="B3" s="0">
-        <v>52.085136006209453</v>
+        <v>37.854275825321153</v>
       </c>
       <c r="C3" s="0">
-        <v>52.086466572421671</v>
+        <v>37.947331922020552</v>
       </c>
       <c r="D3" s="0">
-        <v>2.8941412907063504</v>
+        <v>2.8198344780763467</v>
       </c>
       <c r="E3" s="0">
-        <v>0.11535017174805474</v>
+        <v>0.12</v>
       </c>
       <c r="F3" s="0">
         <v>3</v>
@@ -135,19 +136,19 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="B4" s="0">
-        <v>39.037952632709306</v>
+        <v>37.854275825321153</v>
       </c>
       <c r="C4" s="0">
-        <v>39.038442591886273</v>
+        <v>37.947331922020552</v>
       </c>
       <c r="D4" s="0">
-        <v>2.8583684391061346</v>
+        <v>2.8198344780763467</v>
       </c>
       <c r="E4" s="0">
-        <v>0.069997084008154756</v>
+        <v>0.12</v>
       </c>
       <c r="F4" s="0">
         <v>3</v>
@@ -155,19 +156,19 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>397</v>
+        <v>360</v>
       </c>
       <c r="B5" s="0">
-        <v>47.263278611630838</v>
+        <v>40.717526290664516</v>
       </c>
       <c r="C5" s="0">
-        <v>47.265209192385896</v>
+        <v>40.80441152620633</v>
       </c>
       <c r="D5" s="0">
-        <v>2.8846930111901083</v>
+        <v>2.8304454991108985</v>
       </c>
       <c r="E5" s="0">
-        <v>0.13894534015456828</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="F5" s="0">
         <v>3</v>
@@ -175,19 +176,19 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>324</v>
+        <v>355</v>
       </c>
       <c r="B6" s="0">
-        <v>38.118516450287721</v>
+        <v>40.150703109571744</v>
       </c>
       <c r="C6" s="0">
-        <v>38.118237105091836</v>
+        <v>40.249223594996216</v>
       </c>
       <c r="D6" s="0">
-        <v>2.8511523791516926</v>
+        <v>2.8306955031622527</v>
       </c>
       <c r="E6" s="0">
-        <v>1.1532976059293779e-16</v>
+        <v>0.12</v>
       </c>
       <c r="F6" s="0">
         <v>3</v>
@@ -195,19 +196,19 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="B7" s="0">
-        <v>38.548028387856704</v>
+        <v>37.854275825321153</v>
       </c>
       <c r="C7" s="0">
-        <v>38.54867053479277</v>
+        <v>37.947331922020552</v>
       </c>
       <c r="D7" s="0">
-        <v>2.8571319423197807</v>
+        <v>2.8198344780763467</v>
       </c>
       <c r="E7" s="0">
-        <v>0.080134071160511661</v>
+        <v>0.12</v>
       </c>
       <c r="F7" s="0">
         <v>3</v>
@@ -215,39 +216,39 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>271</v>
+        <v>355</v>
       </c>
       <c r="B8" s="0">
-        <v>31.590800846667001</v>
+        <v>40.150703109571744</v>
       </c>
       <c r="C8" s="0">
-        <v>31.591137997862628</v>
+        <v>40.249223594996216</v>
       </c>
       <c r="D8" s="0">
-        <v>2.826306404258732</v>
+        <v>2.8306955031622527</v>
       </c>
       <c r="E8" s="0">
-        <v>0.058064722132270798</v>
+        <v>0.12</v>
       </c>
       <c r="F8" s="0">
-        <v>3.0000000000000004</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>398</v>
+        <v>336</v>
       </c>
       <c r="B9" s="0">
-        <v>47.276475638366136</v>
+        <v>37.854275825321153</v>
       </c>
       <c r="C9" s="0">
-        <v>47.275786614291256</v>
+        <v>37.947331922020552</v>
       </c>
       <c r="D9" s="0">
-        <v>2.8777298448023609</v>
+        <v>2.8198344780763467</v>
       </c>
       <c r="E9" s="0">
-        <v>6.9475621070419448e-17</v>
+        <v>0.12</v>
       </c>
       <c r="F9" s="0">
         <v>3</v>
@@ -255,79 +256,79 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>311</v>
+        <v>336</v>
       </c>
       <c r="B10" s="0">
-        <v>36.550992882712066</v>
+        <v>37.854275825321153</v>
       </c>
       <c r="C10" s="0">
-        <v>36.551333764994126</v>
+        <v>37.947331922020552</v>
       </c>
       <c r="D10" s="0">
-        <v>2.8486629003212944</v>
+        <v>2.8198344780763467</v>
       </c>
       <c r="E10" s="0">
-        <v>0.058385124995159181</v>
+        <v>0.12</v>
       </c>
       <c r="F10" s="0">
-        <v>3.0000000000000004</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>312</v>
+        <v>355</v>
       </c>
       <c r="B11" s="0">
-        <v>36.726645511645472</v>
+        <v>40.150703109571744</v>
       </c>
       <c r="C11" s="0">
-        <v>36.72873534441392</v>
+        <v>40.249223594996216</v>
       </c>
       <c r="D11" s="0">
-        <v>2.8535673096927385</v>
+        <v>2.8306955031622527</v>
       </c>
       <c r="E11" s="0">
-        <v>0.14456253900839833</v>
+        <v>0.12</v>
       </c>
       <c r="F11" s="0">
-        <v>3.0000000000000004</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>130</v>
+        <v>374</v>
       </c>
       <c r="B12" s="0">
-        <v>14.140817296314848</v>
+        <v>42.352544593482222</v>
       </c>
       <c r="C12" s="0">
-        <v>14.142135623730951</v>
+        <v>42.426406871192853</v>
       </c>
       <c r="D12" s="0">
-        <v>2.6449007310753219</v>
+        <v>2.8336362858726258</v>
       </c>
       <c r="E12" s="0">
-        <v>0.11481843998699208</v>
+        <v>0.12</v>
       </c>
       <c r="F12" s="0">
-        <v>3.0000000000000004</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>121</v>
+        <v>407</v>
       </c>
       <c r="B13" s="0">
-        <v>12.9614731934736</v>
+        <v>44.642305938821906</v>
       </c>
       <c r="C13" s="0">
-        <v>12.961481396815721</v>
+        <v>37.947331922020552</v>
       </c>
       <c r="D13" s="0">
-        <v>2.604503435415332</v>
+        <v>2.742104558963673</v>
       </c>
       <c r="E13" s="0">
-        <v>0.0090572303284447847</v>
+        <v>0</v>
       </c>
       <c r="F13" s="0">
         <v>3.0000000000000004</v>
@@ -335,59 +336,59 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>234</v>
+        <v>360</v>
       </c>
       <c r="B14" s="0">
-        <v>26.999719901796396</v>
+        <v>40.717526290664516</v>
       </c>
       <c r="C14" s="0">
-        <v>27.000000000000004</v>
+        <v>40.804411526206337</v>
       </c>
       <c r="D14" s="0">
-        <v>2.7984905507539182</v>
+        <v>2.8304454991108989</v>
       </c>
       <c r="E14" s="0">
-        <v>0.05292430477606113</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="F14" s="0">
-        <v>3</v>
+        <v>3.0000000000000004</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>474</v>
+        <v>345</v>
       </c>
       <c r="B15" s="0">
-        <v>56.753671036686733</v>
+        <v>38.914142727222959</v>
       </c>
       <c r="C15" s="0">
-        <v>56.753854494650845</v>
+        <v>39</v>
       </c>
       <c r="D15" s="0">
-        <v>2.9001799828926993</v>
+        <v>2.8228186566872711</v>
       </c>
       <c r="E15" s="0">
-        <v>0.042831993196215917</v>
+        <v>0.12</v>
       </c>
       <c r="F15" s="0">
-        <v>3</v>
+        <v>3.0000000000000004</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>405</v>
+        <v>355</v>
       </c>
       <c r="B16" s="0">
-        <v>48.227756781186521</v>
+        <v>40.150703109571744</v>
       </c>
       <c r="C16" s="0">
-        <v>48.228622207149975</v>
+        <v>40.249223594996216</v>
       </c>
       <c r="D16" s="0">
-        <v>2.8851566725257207</v>
+        <v>2.8306955031622527</v>
       </c>
       <c r="E16" s="0">
-        <v>0.093028273307309992</v>
+        <v>0.12</v>
       </c>
       <c r="F16" s="0">
         <v>3</v>
@@ -395,19 +396,19 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>389</v>
+        <v>360</v>
       </c>
       <c r="B17" s="0">
-        <v>46.195223714314857</v>
+        <v>40.717526290664516</v>
       </c>
       <c r="C17" s="0">
-        <v>46.195237849804386</v>
+        <v>40.80441152620633</v>
       </c>
       <c r="D17" s="0">
-        <v>2.8770957028887905</v>
+        <v>2.8304454991108985</v>
       </c>
       <c r="E17" s="0">
-        <v>0.011889276483726558</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="F17" s="0">
         <v>3</v>
@@ -415,19 +416,19 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="B18" s="0">
-        <v>43.462625643645175</v>
+        <v>40.717526290664516</v>
       </c>
       <c r="C18" s="0">
-        <v>43.46262762420146</v>
+        <v>40.80441152620633</v>
       </c>
       <c r="D18" s="0">
-        <v>2.8694038297166493</v>
+        <v>2.8304454991108985</v>
       </c>
       <c r="E18" s="0">
-        <v>0.0044503441256445869</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="F18" s="0">
         <v>3</v>
@@ -435,119 +436,119 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>412</v>
+        <v>367</v>
       </c>
       <c r="B19" s="0">
-        <v>49.050961701364486</v>
+        <v>41.581794270533862</v>
       </c>
       <c r="C19" s="0">
-        <v>49.050993873722888</v>
+        <v>41.677331968349414</v>
       </c>
       <c r="D19" s="0">
-        <v>2.8841917147480816</v>
+        <v>2.8355922083514375</v>
       </c>
       <c r="E19" s="0">
-        <v>0.017936654763098085</v>
+        <v>0.12</v>
       </c>
       <c r="F19" s="0">
-        <v>3</v>
+        <v>3.0000000000000004</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>430</v>
+        <v>340</v>
       </c>
       <c r="B20" s="0">
-        <v>51.312314009667666</v>
+        <v>38.327800470486821</v>
       </c>
       <c r="C20" s="0">
-        <v>51.312766442670004</v>
+        <v>38.418745424597091</v>
       </c>
       <c r="D20" s="0">
-        <v>2.8908749075405749</v>
+        <v>2.82145262403079</v>
       </c>
       <c r="E20" s="0">
-        <v>0.067263140152938883</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="F20" s="0">
-        <v>3.0000000000000004</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>321</v>
+        <v>405</v>
       </c>
       <c r="B21" s="0">
-        <v>37.762404018984142</v>
+        <v>44.414460494040242</v>
       </c>
       <c r="C21" s="0">
-        <v>37.76241517699841</v>
+        <v>39.458839313897712</v>
       </c>
       <c r="D21" s="0">
-        <v>2.8509938018805006</v>
+        <v>2.7418102674217817</v>
       </c>
       <c r="E21" s="0">
-        <v>0.010563150227534858</v>
+        <v>0</v>
       </c>
       <c r="F21" s="0">
-        <v>3.0000000000000004</v>
+        <v>3.0000000000000009</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B22" s="0">
-        <v>39.345228696552859</v>
+        <v>37.014741709153405</v>
       </c>
       <c r="C22" s="0">
-        <v>39.344631145812002</v>
+        <v>37.107950630558946</v>
       </c>
       <c r="D22" s="0">
-        <v>2.8546454590705141</v>
+        <v>2.8160384531148899</v>
       </c>
       <c r="E22" s="0">
-        <v>1.7142473842642453e-15</v>
+        <v>0.12</v>
       </c>
       <c r="F22" s="0">
-        <v>3.0000000000000004</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>197</v>
+        <v>338</v>
       </c>
       <c r="B23" s="0">
-        <v>22.448633042957152</v>
+        <v>38.091589004017067</v>
       </c>
       <c r="C23" s="0">
-        <v>22.449944320643649</v>
+        <v>38.183766184073569</v>
       </c>
       <c r="D23" s="0">
-        <v>2.7656455661980166</v>
+        <v>2.82069124909671</v>
       </c>
       <c r="E23" s="0">
-        <v>0.1145110338130839</v>
+        <v>0.12</v>
       </c>
       <c r="F23" s="0">
-        <v>3.0000000000000004</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>201</v>
+        <v>329</v>
       </c>
       <c r="B24" s="0">
-        <v>22.890986514115113</v>
+        <v>37.014741709153405</v>
       </c>
       <c r="C24" s="0">
-        <v>22.891046284519192</v>
+        <v>37.107950630558946</v>
       </c>
       <c r="D24" s="0">
-        <v>2.7631401382237049</v>
+        <v>2.8160384531148899</v>
       </c>
       <c r="E24" s="0">
-        <v>0.024447986435291103</v>
+        <v>0.12</v>
       </c>
       <c r="F24" s="0">
         <v>3</v>
@@ -555,59 +556,59 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>205</v>
+        <v>329</v>
       </c>
       <c r="B25" s="0">
-        <v>23.45036912477018</v>
+        <v>37.014741709153405</v>
       </c>
       <c r="C25" s="0">
-        <v>23.45207879911715</v>
+        <v>37.107950630558946</v>
       </c>
       <c r="D25" s="0">
-        <v>2.7760588890582101</v>
+        <v>2.8160384531148899</v>
       </c>
       <c r="E25" s="0">
-        <v>0.13075451605831634</v>
+        <v>0.12</v>
       </c>
       <c r="F25" s="0">
-        <v>3.0000000000000004</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>121</v>
+        <v>355</v>
       </c>
       <c r="B26" s="0">
-        <v>13.03659657290957</v>
+        <v>40.150703109571744</v>
       </c>
       <c r="C26" s="0">
-        <v>13.038404810405298</v>
+        <v>40.249223594996216</v>
       </c>
       <c r="D26" s="0">
-        <v>2.6210870375618436</v>
+        <v>2.8306955031622527</v>
       </c>
       <c r="E26" s="0">
-        <v>0.13447072156144244</v>
+        <v>0.12</v>
       </c>
       <c r="F26" s="0">
-        <v>3.0000000000000004</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>133</v>
+        <v>346</v>
       </c>
       <c r="B27" s="0">
-        <v>14.456788646018188</v>
+        <v>39.030456513603106</v>
       </c>
       <c r="C27" s="0">
-        <v>14.456832294800961</v>
+        <v>39.11521443121589</v>
       </c>
       <c r="D27" s="0">
-        <v>2.641611102689664</v>
+        <v>2.8230509495216856</v>
       </c>
       <c r="E27" s="0">
-        <v>0.020892291107833368</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="F27" s="0">
         <v>3</v>
@@ -615,19 +616,19 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="B28" s="0">
-        <v>42.237344287847037</v>
+        <v>39.377801625676319</v>
       </c>
       <c r="C28" s="0">
-        <v>42.237424163885748</v>
+        <v>39.458839313897712</v>
       </c>
       <c r="D28" s="0">
-        <v>2.8668128783993549</v>
+        <v>2.8236197206948468</v>
       </c>
       <c r="E28" s="0">
-        <v>0.028262349285619551</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="F28" s="0">
         <v>3</v>
@@ -635,19 +636,19 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>422</v>
+        <v>346</v>
       </c>
       <c r="B29" s="0">
-        <v>50.328269517815841</v>
+        <v>39.030456513603106</v>
       </c>
       <c r="C29" s="0">
-        <v>50.328918128646478</v>
+        <v>39.11521443121589</v>
       </c>
       <c r="D29" s="0">
-        <v>2.8893094361621428</v>
+        <v>2.8230509495216856</v>
       </c>
       <c r="E29" s="0">
-        <v>0.080536378776520215</v>
+        <v>0.12</v>
       </c>
       <c r="F29" s="0">
         <v>3.0000000000000004</v>
@@ -655,19 +656,19 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>394</v>
+        <v>374</v>
       </c>
       <c r="B30" s="0">
-        <v>46.787304175066751</v>
+        <v>42.352544593482222</v>
       </c>
       <c r="C30" s="0">
-        <v>46.786750261158339</v>
+        <v>42.426406871192853</v>
       </c>
       <c r="D30" s="0">
-        <v>2.8769082364232332</v>
+        <v>2.8336362858726258</v>
       </c>
       <c r="E30" s="0">
-        <v>1.0794385653450954e-16</v>
+        <v>0.12</v>
       </c>
       <c r="F30" s="0">
         <v>3</v>
@@ -675,59 +676,59 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>405</v>
+        <v>356</v>
       </c>
       <c r="B31" s="0">
-        <v>48.187074742271996</v>
+        <v>40.264450051296137</v>
       </c>
       <c r="C31" s="0">
-        <v>48.187135212627034</v>
+        <v>40.360872141221137</v>
       </c>
       <c r="D31" s="0">
-        <v>2.8824529667483008</v>
+        <v>2.8307086104174863</v>
       </c>
       <c r="E31" s="0">
-        <v>0.024590720816361104</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="F31" s="0">
-        <v>3</v>
+        <v>2.9999999999999996</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>292</v>
+        <v>356</v>
       </c>
       <c r="B32" s="0">
-        <v>34.233002009577234</v>
+        <v>40.264450051296137</v>
       </c>
       <c r="C32" s="0">
-        <v>34.23448553724738</v>
+        <v>40.360872141221137</v>
       </c>
       <c r="D32" s="0">
-        <v>2.8422904192143994</v>
+        <v>2.8307086104174863</v>
       </c>
       <c r="E32" s="0">
-        <v>0.12180015066279333</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="F32" s="0">
-        <v>3.0000000000000004</v>
+        <v>2.9999999999999996</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>173</v>
+        <v>370</v>
       </c>
       <c r="B33" s="0">
-        <v>19.391089644777111</v>
+        <v>41.914142727222931</v>
       </c>
       <c r="C33" s="0">
-        <v>19.390719429665317</v>
+        <v>42</v>
       </c>
       <c r="D33" s="0">
-        <v>2.7207536694282335</v>
+        <v>2.8347903690732701</v>
       </c>
       <c r="E33" s="0">
-        <v>4.3994995102956563e-16</v>
+        <v>0.12</v>
       </c>
       <c r="F33" s="0">
         <v>3</v>
@@ -735,19 +736,19 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>287</v>
+        <v>399</v>
       </c>
       <c r="B34" s="0">
-        <v>33.613950309367027</v>
+        <v>43.776869834440468</v>
       </c>
       <c r="C34" s="0">
-        <v>33.615472627943227</v>
+        <v>39</v>
       </c>
       <c r="D34" s="0">
-        <v>2.8396310675908221</v>
+        <v>2.7430210962483708</v>
       </c>
       <c r="E34" s="0">
-        <v>0.12338227491036961</v>
+        <v>1.3877787807814457e-17</v>
       </c>
       <c r="F34" s="0">
         <v>3.0000000000000004</v>
@@ -755,39 +756,39 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>178</v>
+        <v>360</v>
       </c>
       <c r="B35" s="0">
-        <v>20.121941570956604</v>
+        <v>40.717526290664516</v>
       </c>
       <c r="C35" s="0">
-        <v>20.124611797498108</v>
+        <v>40.804411526206337</v>
       </c>
       <c r="D35" s="0">
-        <v>2.7450254632174409</v>
+        <v>2.8304454991108989</v>
       </c>
       <c r="E35" s="0">
-        <v>0.16340827829403215</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="F35" s="0">
-        <v>3</v>
+        <v>3.0000000000000004</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>164</v>
+        <v>368</v>
       </c>
       <c r="B36" s="0">
-        <v>18.356262589738748</v>
+        <v>41.692643274219272</v>
       </c>
       <c r="C36" s="0">
-        <v>18.357559750685819</v>
+        <v>41.785164831552358</v>
       </c>
       <c r="D36" s="0">
-        <v>2.7184285828053518</v>
+        <v>2.8353842405564209</v>
       </c>
       <c r="E36" s="0">
-        <v>0.11389297375485632</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="F36" s="0">
         <v>3</v>
@@ -795,39 +796,39 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>271</v>
+        <v>375</v>
       </c>
       <c r="B37" s="0">
-        <v>31.63676809725084</v>
+        <v>42.542304064188741</v>
       </c>
       <c r="C37" s="0">
-        <v>31.63858403911275</v>
+        <v>42.638011210655691</v>
       </c>
       <c r="D37" s="0">
-        <v>2.8308343549575441</v>
+        <v>2.8391353679479621</v>
       </c>
       <c r="E37" s="0">
-        <v>0.13475688709341072</v>
+        <v>0.12</v>
       </c>
       <c r="F37" s="0">
-        <v>3</v>
+        <v>2.9999999999999996</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>282</v>
+        <v>338</v>
       </c>
       <c r="B38" s="0">
-        <v>32.909278229674456</v>
+        <v>38.091589004017067</v>
       </c>
       <c r="C38" s="0">
-        <v>32.908965343808674</v>
+        <v>38.183766184073569</v>
       </c>
       <c r="D38" s="0">
-        <v>2.8288772525484331</v>
+        <v>2.82069124909671</v>
       </c>
       <c r="E38" s="0">
-        <v>3.9178644255214178e-16</v>
+        <v>0.12</v>
       </c>
       <c r="F38" s="0">
         <v>3</v>
@@ -835,39 +836,39 @@
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>377</v>
+        <v>338</v>
       </c>
       <c r="B39" s="0">
-        <v>44.732248972962502</v>
+        <v>38.091589004017067</v>
       </c>
       <c r="C39" s="0">
-        <v>44.732538492690082</v>
+        <v>38.183766184073569</v>
       </c>
       <c r="D39" s="0">
-        <v>2.8749626328878195</v>
+        <v>2.82069124909671</v>
       </c>
       <c r="E39" s="0">
-        <v>0.053807037419249457</v>
+        <v>0.12</v>
       </c>
       <c r="F39" s="0">
-        <v>3.0000000000000004</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>377</v>
+        <v>360</v>
       </c>
       <c r="B40" s="0">
-        <v>44.754074023073741</v>
+        <v>40.717526290664516</v>
       </c>
       <c r="C40" s="0">
-        <v>44.754888001200499</v>
+        <v>40.804411526206337</v>
       </c>
       <c r="D40" s="0">
-        <v>2.8765080418610292</v>
+        <v>2.8304454991108989</v>
       </c>
       <c r="E40" s="0">
-        <v>0.090220736350513725</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="F40" s="0">
         <v>3.0000000000000004</v>
@@ -875,19 +876,19 @@
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>437</v>
+        <v>360</v>
       </c>
       <c r="B41" s="0">
-        <v>52.153570150104045</v>
+        <v>40.717526290664516</v>
       </c>
       <c r="C41" s="0">
-        <v>52.153619241621193</v>
+        <v>40.804411526206337</v>
       </c>
       <c r="D41" s="0">
-        <v>2.8909714089005418</v>
+        <v>2.8304454991108989</v>
       </c>
       <c r="E41" s="0">
-        <v>0.022156605596047995</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="F41" s="0">
         <v>3.0000000000000004</v>
@@ -895,79 +896,79 @@
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>429</v>
+        <v>321</v>
       </c>
       <c r="B42" s="0">
-        <v>51.146879297771171</v>
+        <v>36.037810617376984</v>
       </c>
       <c r="C42" s="0">
-        <v>51.146847410177685</v>
+        <v>36.124783736376884</v>
       </c>
       <c r="D42" s="0">
-        <v>2.8880556889269964</v>
+        <v>2.8098681650359376</v>
       </c>
       <c r="E42" s="0">
-        <v>1.5531346546082258e-16</v>
+        <v>0.12</v>
       </c>
       <c r="F42" s="0">
-        <v>3</v>
+        <v>3.0000000000000004</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>475</v>
+        <v>360</v>
       </c>
       <c r="B43" s="0">
-        <v>56.833592160560556</v>
+        <v>40.717526290664516</v>
       </c>
       <c r="C43" s="0">
-        <v>56.833088953531288</v>
+        <v>40.80441152620633</v>
       </c>
       <c r="D43" s="0">
-        <v>2.8980152697506187</v>
+        <v>2.8304454991108985</v>
       </c>
       <c r="E43" s="0">
-        <v>4.0466306172113696e-16</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="F43" s="0">
-        <v>3.0000000000000004</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>490</v>
+        <v>363</v>
       </c>
       <c r="B44" s="0">
-        <v>58.702909029972588</v>
+        <v>39.478674852878683</v>
       </c>
       <c r="C44" s="0">
-        <v>58.702640485756689</v>
+        <v>37.107950630558946</v>
       </c>
       <c r="D44" s="0">
-        <v>2.9015977098472248</v>
+        <v>2.718863965257424</v>
       </c>
       <c r="E44" s="0">
-        <v>2.5362582704159623e-16</v>
+        <v>0</v>
       </c>
       <c r="F44" s="0">
-        <v>3</v>
+        <v>3.0000000000000009</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>233</v>
+        <v>346</v>
       </c>
       <c r="B45" s="0">
-        <v>26.86987135288032</v>
+        <v>39.030456513603106</v>
       </c>
       <c r="C45" s="0">
-        <v>26.870057685088806</v>
+        <v>39.11521443121589</v>
       </c>
       <c r="D45" s="0">
-        <v>2.7969556198882337</v>
+        <v>2.8230509495216856</v>
       </c>
       <c r="E45" s="0">
-        <v>0.043166214622400251</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="F45" s="0">
         <v>3</v>
@@ -975,39 +976,39 @@
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>217</v>
+        <v>439</v>
       </c>
       <c r="B46" s="0">
-        <v>24.918905655855859</v>
+        <v>48.556993525570398</v>
       </c>
       <c r="C46" s="0">
-        <v>24.919871588754223</v>
+        <v>40.249223594996216</v>
       </c>
       <c r="D46" s="0">
-        <v>2.7860484339412261</v>
+        <v>2.7654356078122051</v>
       </c>
       <c r="E46" s="0">
-        <v>0.098281885327884969</v>
+        <v>1.3877787807814457e-17</v>
       </c>
       <c r="F46" s="0">
-        <v>3</v>
+        <v>3.0000000000000009</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>210</v>
+        <v>346</v>
       </c>
       <c r="B47" s="0">
-        <v>24.020596643311659</v>
+        <v>39.030456513603106</v>
       </c>
       <c r="C47" s="0">
-        <v>24.020824298928627</v>
+        <v>39.11521443121589</v>
       </c>
       <c r="D47" s="0">
-        <v>2.7750638682188371</v>
+        <v>2.8230509495216856</v>
       </c>
       <c r="E47" s="0">
-        <v>0.047713270372233052</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="F47" s="0">
         <v>3</v>
@@ -1015,19 +1016,19 @@
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>325</v>
+        <v>407</v>
       </c>
       <c r="B48" s="0">
-        <v>38.275168978709509</v>
+        <v>44.698600785402512</v>
       </c>
       <c r="C48" s="0">
-        <v>38.275318418009277</v>
+        <v>39</v>
       </c>
       <c r="D48" s="0">
-        <v>2.8542108248419966</v>
+        <v>2.7459909932040585</v>
       </c>
       <c r="E48" s="0">
-        <v>0.038657379603046542</v>
+        <v>0</v>
       </c>
       <c r="F48" s="0">
         <v>3.0000000000000004</v>
@@ -1035,19 +1036,19 @@
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B49" s="0">
-        <v>41.772541215483173</v>
+        <v>38.327800470486821</v>
       </c>
       <c r="C49" s="0">
-        <v>41.773197148410844</v>
+        <v>38.418745424597091</v>
       </c>
       <c r="D49" s="0">
-        <v>2.8676935835121569</v>
+        <v>2.82145262403079</v>
       </c>
       <c r="E49" s="0">
-        <v>0.080989686236955696</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="F49" s="0">
         <v>3</v>
@@ -1055,602 +1056,2639 @@
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="B50" s="0">
-        <v>0</v>
+        <v>40.717526290664516</v>
       </c>
       <c r="C50" s="0">
-        <v>0</v>
+        <v>40.804411526206337</v>
       </c>
       <c r="D50" s="0">
-        <v>0</v>
+        <v>2.8304454991108989</v>
       </c>
       <c r="E50" s="0">
-        <v>0</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="F50" s="0">
-        <v>0</v>
+        <v>3.0000000000000004</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="B51" s="0">
-        <v>0</v>
+        <v>38.327800470486821</v>
       </c>
       <c r="C51" s="0">
-        <v>0</v>
+        <v>38.418745424597091</v>
       </c>
       <c r="D51" s="0">
-        <v>0</v>
+        <v>2.82145262403079</v>
       </c>
       <c r="E51" s="0">
-        <v>0</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="F51" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>0</v>
+        <v>356</v>
       </c>
       <c r="B52" s="0">
-        <v>0</v>
+        <v>40.264450051296137</v>
       </c>
       <c r="C52" s="0">
-        <v>0</v>
+        <v>40.360872141221137</v>
       </c>
       <c r="D52" s="0">
-        <v>0</v>
+        <v>2.8307086104174863</v>
       </c>
       <c r="E52" s="0">
-        <v>0</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="F52" s="0">
-        <v>0</v>
+        <v>2.9999999999999996</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="B53" s="0">
-        <v>0</v>
+        <v>38.327800470486821</v>
       </c>
       <c r="C53" s="0">
-        <v>0</v>
+        <v>38.418745424597091</v>
       </c>
       <c r="D53" s="0">
-        <v>0</v>
+        <v>2.82145262403079</v>
       </c>
       <c r="E53" s="0">
-        <v>0</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="F53" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="B54" s="0">
-        <v>0</v>
+        <v>38.327800470486821</v>
       </c>
       <c r="C54" s="0">
-        <v>0</v>
+        <v>38.418745424597091</v>
       </c>
       <c r="D54" s="0">
-        <v>0</v>
+        <v>2.82145262403079</v>
       </c>
       <c r="E54" s="0">
-        <v>0</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="F54" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>0</v>
+        <v>345</v>
       </c>
       <c r="B55" s="0">
-        <v>0</v>
+        <v>38.914142727222959</v>
       </c>
       <c r="C55" s="0">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="D55" s="0">
-        <v>0</v>
+        <v>2.8228186566872711</v>
       </c>
       <c r="E55" s="0">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F55" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="B56" s="0">
-        <v>0</v>
+        <v>40.717526290664516</v>
       </c>
       <c r="C56" s="0">
-        <v>0</v>
+        <v>40.80441152620633</v>
       </c>
       <c r="D56" s="0">
-        <v>0</v>
+        <v>2.8304454991108985</v>
       </c>
       <c r="E56" s="0">
-        <v>0</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="F56" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>0</v>
+        <v>321</v>
       </c>
       <c r="B57" s="0">
-        <v>0</v>
+        <v>36.037810617376984</v>
       </c>
       <c r="C57" s="0">
-        <v>0</v>
+        <v>36.124783736376884</v>
       </c>
       <c r="D57" s="0">
-        <v>0</v>
+        <v>2.8098681650359376</v>
       </c>
       <c r="E57" s="0">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F57" s="0">
-        <v>0</v>
+        <v>3.0000000000000004</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>0</v>
+        <v>398</v>
       </c>
       <c r="B58" s="0">
-        <v>0</v>
+        <v>43.628171319749534</v>
       </c>
       <c r="C58" s="0">
-        <v>0</v>
+        <v>40.804411526206337</v>
       </c>
       <c r="D58" s="0">
-        <v>0</v>
+        <v>2.7407821886293542</v>
       </c>
       <c r="E58" s="0">
         <v>0</v>
       </c>
       <c r="F58" s="0">
-        <v>0</v>
+        <v>3.0000000000000009</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="B59" s="0">
-        <v>0</v>
+        <v>40.717526290664516</v>
       </c>
       <c r="C59" s="0">
-        <v>0</v>
+        <v>40.804411526206337</v>
       </c>
       <c r="D59" s="0">
-        <v>0</v>
+        <v>2.8304454991108989</v>
       </c>
       <c r="E59" s="0">
-        <v>0</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="F59" s="0">
-        <v>0</v>
+        <v>3.0000000000000004</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>0</v>
+        <v>375</v>
       </c>
       <c r="B60" s="0">
-        <v>0</v>
+        <v>42.542304064188741</v>
       </c>
       <c r="C60" s="0">
-        <v>0</v>
+        <v>42.638011210655691</v>
       </c>
       <c r="D60" s="0">
-        <v>0</v>
+        <v>2.8391353679479621</v>
       </c>
       <c r="E60" s="0">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F60" s="0">
-        <v>0</v>
+        <v>2.9999999999999996</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>0</v>
+        <v>443</v>
       </c>
       <c r="B61" s="0">
-        <v>0</v>
+        <v>49.02359643035215</v>
       </c>
       <c r="C61" s="0">
-        <v>0</v>
+        <v>40.804411526206337</v>
       </c>
       <c r="D61" s="0">
-        <v>0</v>
+        <v>2.7668854022399234</v>
       </c>
       <c r="E61" s="0">
         <v>0</v>
       </c>
       <c r="F61" s="0">
-        <v>0</v>
+        <v>3.0000000000000009</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B62" s="0">
-        <v>0</v>
+        <v>49.332610326702365</v>
       </c>
       <c r="C62" s="0">
-        <v>0</v>
+        <v>39.458839313897712</v>
       </c>
       <c r="D62" s="0">
-        <v>0</v>
+        <v>2.7654299658490169</v>
       </c>
       <c r="E62" s="0">
         <v>0</v>
       </c>
       <c r="F62" s="0">
-        <v>0</v>
+        <v>3.0000000000000009</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0">
-        <v>0</v>
+        <v>349</v>
       </c>
       <c r="B63" s="0">
-        <v>0</v>
+        <v>39.377801625676319</v>
       </c>
       <c r="C63" s="0">
-        <v>0</v>
+        <v>39.458839313897712</v>
       </c>
       <c r="D63" s="0">
-        <v>0</v>
+        <v>2.8236197206948468</v>
       </c>
       <c r="E63" s="0">
-        <v>0</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="F63" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0">
+        <v>338</v>
+      </c>
+      <c r="B64" s="0">
+        <v>38.091589004017067</v>
+      </c>
+      <c r="C64" s="0">
+        <v>38.183766184073569</v>
+      </c>
+      <c r="D64" s="0">
+        <v>2.82069124909671</v>
+      </c>
+      <c r="E64" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F64" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0">
+        <v>354</v>
+      </c>
+      <c r="B65" s="0">
+        <v>39.951436974065551</v>
+      </c>
+      <c r="C65" s="0">
+        <v>40.024992192379003</v>
+      </c>
+      <c r="D65" s="0">
+        <v>2.8241550338051082</v>
+      </c>
+      <c r="E65" s="0">
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F65" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="0">
+        <v>355</v>
+      </c>
+      <c r="B66" s="0">
+        <v>40.150703109571744</v>
+      </c>
+      <c r="C66" s="0">
+        <v>40.249223594996216</v>
+      </c>
+      <c r="D66" s="0">
+        <v>2.8306955031622527</v>
+      </c>
+      <c r="E66" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F66" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="0">
+        <v>345</v>
+      </c>
+      <c r="B67" s="0">
+        <v>38.914142727222959</v>
+      </c>
+      <c r="C67" s="0">
+        <v>39</v>
+      </c>
+      <c r="D67" s="0">
+        <v>2.8228186566872711</v>
+      </c>
+      <c r="E67" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F67" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="0">
+        <v>349</v>
+      </c>
+      <c r="B68" s="0">
+        <v>39.377801625676319</v>
+      </c>
+      <c r="C68" s="0">
+        <v>39.458839313897712</v>
+      </c>
+      <c r="D68" s="0">
+        <v>2.8236197206948468</v>
+      </c>
+      <c r="E68" s="0">
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F68" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="0">
+        <v>368</v>
+      </c>
+      <c r="B69" s="0">
+        <v>41.692643274219272</v>
+      </c>
+      <c r="C69" s="0">
+        <v>41.785164831552358</v>
+      </c>
+      <c r="D69" s="0">
+        <v>2.8353842405564209</v>
+      </c>
+      <c r="E69" s="0">
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F69" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="0">
+        <v>449</v>
+      </c>
+      <c r="B70" s="0">
+        <v>49.799705684842792</v>
+      </c>
+      <c r="C70" s="0">
+        <v>37.107950630558946</v>
+      </c>
+      <c r="D70" s="0">
+        <v>2.7727651522355736</v>
+      </c>
+      <c r="E70" s="0">
         <v>0</v>
       </c>
+      <c r="F70" s="0">
+        <v>3.0000000000000009</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="0">
+        <v>340</v>
+      </c>
+      <c r="B71" s="0">
+        <v>38.327800470486821</v>
+      </c>
+      <c r="C71" s="0">
+        <v>38.418745424597091</v>
+      </c>
+      <c r="D71" s="0">
+        <v>2.82145262403079</v>
+      </c>
+      <c r="E71" s="0">
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F71" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="0">
+        <v>346</v>
+      </c>
+      <c r="B72" s="0">
+        <v>39.030456513603106</v>
+      </c>
+      <c r="C72" s="0">
+        <v>39.11521443121589</v>
+      </c>
+      <c r="D72" s="0">
+        <v>2.8230509495216856</v>
+      </c>
+      <c r="E72" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F72" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="0">
+        <v>321</v>
+      </c>
+      <c r="B73" s="0">
+        <v>36.037810617376984</v>
+      </c>
+      <c r="C73" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D73" s="0">
+        <v>2.8098681650359376</v>
+      </c>
+      <c r="E73" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F73" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="0">
+        <v>345</v>
+      </c>
+      <c r="B74" s="0">
+        <v>38.914142727222959</v>
+      </c>
+      <c r="C74" s="0">
+        <v>39</v>
+      </c>
+      <c r="D74" s="0">
+        <v>2.8228186566872711</v>
+      </c>
+      <c r="E74" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F74" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="0">
+        <v>354</v>
+      </c>
+      <c r="B75" s="0">
+        <v>39.951436974065551</v>
+      </c>
+      <c r="C75" s="0">
+        <v>40.024992192379003</v>
+      </c>
+      <c r="D75" s="0">
+        <v>2.8241550338051082</v>
+      </c>
+      <c r="E75" s="0">
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F75" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="0">
+        <v>471</v>
+      </c>
+      <c r="B76" s="0">
+        <v>52.419579297083075</v>
+      </c>
+      <c r="C76" s="0">
+        <v>45.09988913511873</v>
+      </c>
+      <c r="D76" s="0">
+        <v>2.7824290899968354</v>
+      </c>
+      <c r="E76" s="0">
+        <v>1.3877787807814455e-17</v>
+      </c>
+      <c r="F76" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="0">
+        <v>345</v>
+      </c>
+      <c r="B77" s="0">
+        <v>38.914142727222959</v>
+      </c>
+      <c r="C77" s="0">
+        <v>39</v>
+      </c>
+      <c r="D77" s="0">
+        <v>2.8228186566872711</v>
+      </c>
+      <c r="E77" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F77" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="0">
+        <v>441</v>
+      </c>
+      <c r="B78" s="0">
+        <v>48.838936115457081</v>
+      </c>
+      <c r="C78" s="0">
+        <v>39.458839313897712</v>
+      </c>
+      <c r="D78" s="0">
+        <v>2.7686052433027433</v>
+      </c>
+      <c r="E78" s="0">
+        <v>0</v>
+      </c>
+      <c r="F78" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="0">
+        <v>346</v>
+      </c>
+      <c r="B79" s="0">
+        <v>39.030456513603106</v>
+      </c>
+      <c r="C79" s="0">
+        <v>39.11521443121589</v>
+      </c>
+      <c r="D79" s="0">
+        <v>2.8230509495216856</v>
+      </c>
+      <c r="E79" s="0">
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F79" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="0">
+        <v>414</v>
+      </c>
+      <c r="B80" s="0">
+        <v>45.567364286769383</v>
+      </c>
+      <c r="C80" s="0">
+        <v>39</v>
+      </c>
+      <c r="D80" s="0">
+        <v>2.751824555372592</v>
+      </c>
+      <c r="E80" s="0">
+        <v>0</v>
+      </c>
+      <c r="F80" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="0">
+        <v>345</v>
+      </c>
+      <c r="B81" s="0">
+        <v>38.914142727222959</v>
+      </c>
+      <c r="C81" s="0">
+        <v>39</v>
+      </c>
+      <c r="D81" s="0">
+        <v>2.8228186566872711</v>
+      </c>
+      <c r="E81" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F81" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="0">
+        <v>345</v>
+      </c>
+      <c r="B82" s="0">
+        <v>38.914142727222959</v>
+      </c>
+      <c r="C82" s="0">
+        <v>39</v>
+      </c>
+      <c r="D82" s="0">
+        <v>2.8228186566872711</v>
+      </c>
+      <c r="E82" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F82" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="0">
+        <v>461</v>
+      </c>
+      <c r="B83" s="0">
+        <v>51.225443488870852</v>
+      </c>
+      <c r="C83" s="0">
+        <v>42.426406871192853</v>
+      </c>
+      <c r="D83" s="0">
+        <v>2.7779936575925017</v>
+      </c>
+      <c r="E83" s="0">
+        <v>0</v>
+      </c>
+      <c r="F83" s="0">
+        <v>3.0000000000000009</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="0">
+        <v>352</v>
+      </c>
+      <c r="B84" s="0">
+        <v>38.121257657276225</v>
+      </c>
+      <c r="C84" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D84" s="0">
+        <v>2.7077259993640794</v>
+      </c>
+      <c r="E84" s="0">
+        <v>0</v>
+      </c>
+      <c r="F84" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="0">
+        <v>432</v>
+      </c>
+      <c r="B85" s="0">
+        <v>47.680118358757539</v>
+      </c>
+      <c r="C85" s="0">
+        <v>40.249223594996216</v>
+      </c>
+      <c r="D85" s="0">
+        <v>2.7595969369680384</v>
+      </c>
+      <c r="E85" s="0">
+        <v>1.3877787807814455e-17</v>
+      </c>
+      <c r="F85" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="0">
+        <v>345</v>
+      </c>
+      <c r="B86" s="0">
+        <v>38.914142727222959</v>
+      </c>
+      <c r="C86" s="0">
+        <v>39</v>
+      </c>
+      <c r="D86" s="0">
+        <v>2.8228186566872711</v>
+      </c>
+      <c r="E86" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F86" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="0">
+        <v>360</v>
+      </c>
+      <c r="B87" s="0">
+        <v>40.717526290664516</v>
+      </c>
+      <c r="C87" s="0">
+        <v>40.80441152620633</v>
+      </c>
+      <c r="D87" s="0">
+        <v>2.8304454991108985</v>
+      </c>
+      <c r="E87" s="0">
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F87" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="0">
+        <v>321</v>
+      </c>
+      <c r="B88" s="0">
+        <v>36.037810617376984</v>
+      </c>
+      <c r="C88" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D88" s="0">
+        <v>2.8098681650359376</v>
+      </c>
+      <c r="E88" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F88" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="0">
+        <v>345</v>
+      </c>
+      <c r="B89" s="0">
+        <v>38.914142727222959</v>
+      </c>
+      <c r="C89" s="0">
+        <v>39</v>
+      </c>
+      <c r="D89" s="0">
+        <v>2.8228186566872711</v>
+      </c>
+      <c r="E89" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F89" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="0">
+        <v>374</v>
+      </c>
+      <c r="B90" s="0">
+        <v>42.352544593482222</v>
+      </c>
+      <c r="C90" s="0">
+        <v>42.426406871192853</v>
+      </c>
+      <c r="D90" s="0">
+        <v>2.8336362858726258</v>
+      </c>
+      <c r="E90" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F90" s="0">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F90"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="3" max="3" width="11.7109375" customWidth="true"/>
+    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+    <col min="5" max="5" width="15.5703125" customWidth="true"/>
+    <col min="6" max="6" width="2.140625" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0">
+        <v>313</v>
+      </c>
+      <c r="B1" s="0">
+        <v>35.038558960558809</v>
+      </c>
+      <c r="C1" s="0">
+        <v>35.114099732158877</v>
+      </c>
+      <c r="D1" s="0">
+        <v>2.8017186055174013</v>
+      </c>
+      <c r="E1" s="0">
+        <v>0.11999999999999998</v>
+      </c>
+      <c r="F1" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>300</v>
+      </c>
+      <c r="B2" s="0">
+        <v>33.468324010364114</v>
+      </c>
+      <c r="C2" s="0">
+        <v>33.541019662496851</v>
+      </c>
+      <c r="D2" s="0">
+        <v>2.7922304247514802</v>
+      </c>
+      <c r="E2" s="0">
+        <v>0.11999999999999998</v>
+      </c>
+      <c r="F2" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>322</v>
+      </c>
+      <c r="B3" s="0">
+        <v>36.161134209563251</v>
+      </c>
+      <c r="C3" s="0">
+        <v>36.24913792078371</v>
+      </c>
+      <c r="D3" s="0">
+        <v>2.8107236898769608</v>
+      </c>
+      <c r="E3" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F3" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>312</v>
+      </c>
+      <c r="B4" s="0">
+        <v>34.912000114313003</v>
+      </c>
+      <c r="C4" s="0">
+        <v>34.985711369071801</v>
+      </c>
+      <c r="D4" s="0">
+        <v>2.8005309983568001</v>
+      </c>
+      <c r="E4" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F4" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>313</v>
+      </c>
+      <c r="B5" s="0">
+        <v>35.038558960558809</v>
+      </c>
+      <c r="C5" s="0">
+        <v>35.114099732158877</v>
+      </c>
+      <c r="D5" s="0">
+        <v>2.8017186055174013</v>
+      </c>
+      <c r="E5" s="0">
+        <v>0.11999999999999998</v>
+      </c>
+      <c r="F5" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>322</v>
+      </c>
+      <c r="B6" s="0">
+        <v>36.161134209563251</v>
+      </c>
+      <c r="C6" s="0">
+        <v>36.24913792078371</v>
+      </c>
+      <c r="D6" s="0">
+        <v>2.8107236898769608</v>
+      </c>
+      <c r="E6" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F6" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>321</v>
+      </c>
+      <c r="B7" s="0">
+        <v>36.037810617376984</v>
+      </c>
+      <c r="C7" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D7" s="0">
+        <v>2.8098681650359376</v>
+      </c>
+      <c r="E7" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F7" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>325</v>
+      </c>
+      <c r="B8" s="0">
+        <v>36.528496220724051</v>
+      </c>
+      <c r="C8" s="0">
+        <v>36.61966684720111</v>
+      </c>
+      <c r="D8" s="0">
+        <v>2.8132683412551933</v>
+      </c>
+      <c r="E8" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F8" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>340</v>
+      </c>
+      <c r="B9" s="0">
+        <v>38.327800470486821</v>
+      </c>
+      <c r="C9" s="0">
+        <v>38.418745424597091</v>
+      </c>
+      <c r="D9" s="0">
+        <v>2.82145262403079</v>
+      </c>
+      <c r="E9" s="0">
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F9" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>321</v>
+      </c>
+      <c r="B10" s="0">
+        <v>36.037810617376984</v>
+      </c>
+      <c r="C10" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D10" s="0">
+        <v>2.8098681650359376</v>
+      </c>
+      <c r="E10" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F10" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>321</v>
+      </c>
+      <c r="B11" s="0">
+        <v>36.037810617376984</v>
+      </c>
+      <c r="C11" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D11" s="0">
+        <v>2.8098681650359376</v>
+      </c>
+      <c r="E11" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F11" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>320</v>
+      </c>
+      <c r="B12" s="0">
+        <v>35.914142727222959</v>
+      </c>
+      <c r="C12" s="0">
+        <v>36</v>
+      </c>
+      <c r="D12" s="0">
+        <v>2.80897636424096</v>
+      </c>
+      <c r="E12" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F12" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>281</v>
+      </c>
+      <c r="B13" s="0">
+        <v>31.234850393355007</v>
+      </c>
+      <c r="C13" s="0">
+        <v>31.32091952673165</v>
+      </c>
+      <c r="D13" s="0">
+        <v>2.7825303252691826</v>
+      </c>
+      <c r="E13" s="0">
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F13" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>346</v>
+      </c>
+      <c r="B14" s="0">
+        <v>39.030456513603106</v>
+      </c>
+      <c r="C14" s="0">
+        <v>39.11521443121589</v>
+      </c>
+      <c r="D14" s="0">
+        <v>2.8230509495216856</v>
+      </c>
+      <c r="E14" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F14" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>320</v>
+      </c>
+      <c r="B15" s="0">
+        <v>35.914142727222959</v>
+      </c>
+      <c r="C15" s="0">
+        <v>36</v>
+      </c>
+      <c r="D15" s="0">
+        <v>2.80897636424096</v>
+      </c>
+      <c r="E15" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F15" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>321</v>
+      </c>
+      <c r="B16" s="0">
+        <v>36.037810617376984</v>
+      </c>
+      <c r="C16" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D16" s="0">
+        <v>2.8098681650359376</v>
+      </c>
+      <c r="E16" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F16" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>340</v>
+      </c>
+      <c r="B17" s="0">
+        <v>38.327800470486821</v>
+      </c>
+      <c r="C17" s="0">
+        <v>38.418745424597091</v>
+      </c>
+      <c r="D17" s="0">
+        <v>2.82145262403079</v>
+      </c>
+      <c r="E17" s="0">
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F17" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>333</v>
+      </c>
+      <c r="B18" s="0">
+        <v>37.496203130873489</v>
+      </c>
+      <c r="C18" s="0">
+        <v>37.589892258425003</v>
+      </c>
+      <c r="D18" s="0">
+        <v>2.8183637519920945</v>
+      </c>
+      <c r="E18" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F18" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>340</v>
+      </c>
+      <c r="B19" s="0">
+        <v>38.327800470486821</v>
+      </c>
+      <c r="C19" s="0">
+        <v>38.418745424597091</v>
+      </c>
+      <c r="D19" s="0">
+        <v>2.82145262403079</v>
+      </c>
+      <c r="E19" s="0">
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F19" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>324</v>
+      </c>
+      <c r="B20" s="0">
+        <v>36.406160922878364</v>
+      </c>
+      <c r="C20" s="0">
+        <v>36.496575181789311</v>
+      </c>
+      <c r="D20" s="0">
+        <v>2.8125022337111707</v>
+      </c>
+      <c r="E20" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F20" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>345</v>
+      </c>
+      <c r="B21" s="0">
+        <v>38.914142727222959</v>
+      </c>
+      <c r="C21" s="0">
+        <v>39</v>
+      </c>
+      <c r="D21" s="0">
+        <v>2.8228186566872711</v>
+      </c>
+      <c r="E21" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F21" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>324</v>
+      </c>
+      <c r="B22" s="0">
+        <v>36.406160922878364</v>
+      </c>
+      <c r="C22" s="0">
+        <v>36.496575181789311</v>
+      </c>
+      <c r="D22" s="0">
+        <v>2.8125022337111707</v>
+      </c>
+      <c r="E22" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F22" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>271</v>
+      </c>
+      <c r="B23" s="0">
+        <v>30.056003428459412</v>
+      </c>
+      <c r="C23" s="0">
+        <v>30.14962686336267</v>
+      </c>
+      <c r="D23" s="0">
+        <v>2.7767891932569149</v>
+      </c>
+      <c r="E23" s="0">
+        <v>0.11999999999999998</v>
+      </c>
+      <c r="F23" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>336</v>
+      </c>
+      <c r="B24" s="0">
+        <v>37.854275825321153</v>
+      </c>
+      <c r="C24" s="0">
+        <v>37.947331922020552</v>
+      </c>
+      <c r="D24" s="0">
+        <v>2.8198344780763467</v>
+      </c>
+      <c r="E24" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F24" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
+        <v>329</v>
+      </c>
+      <c r="B25" s="0">
+        <v>37.014741709153405</v>
+      </c>
+      <c r="C25" s="0">
+        <v>37.107950630558946</v>
+      </c>
+      <c r="D25" s="0">
+        <v>2.8160384531148899</v>
+      </c>
+      <c r="E25" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F25" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
+        <v>336</v>
+      </c>
+      <c r="B26" s="0">
+        <v>37.854275825321153</v>
+      </c>
+      <c r="C26" s="0">
+        <v>37.947331922020552</v>
+      </c>
+      <c r="D26" s="0">
+        <v>2.8198344780763467</v>
+      </c>
+      <c r="E26" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F26" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0">
+        <v>320</v>
+      </c>
+      <c r="B27" s="0">
+        <v>35.914142727222959</v>
+      </c>
+      <c r="C27" s="0">
+        <v>36</v>
+      </c>
+      <c r="D27" s="0">
+        <v>2.80897636424096</v>
+      </c>
+      <c r="E27" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F27" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>349</v>
+      </c>
+      <c r="B28" s="0">
+        <v>39.377801625676319</v>
+      </c>
+      <c r="C28" s="0">
+        <v>39.458839313897712</v>
+      </c>
+      <c r="D28" s="0">
+        <v>2.8236197206948468</v>
+      </c>
+      <c r="E28" s="0">
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F28" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0">
+        <v>329</v>
+      </c>
+      <c r="B29" s="0">
+        <v>37.014741709153405</v>
+      </c>
+      <c r="C29" s="0">
+        <v>37.107950630558946</v>
+      </c>
+      <c r="D29" s="0">
+        <v>2.8160384531148899</v>
+      </c>
+      <c r="E29" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F29" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0">
+        <v>313</v>
+      </c>
+      <c r="B30" s="0">
+        <v>35.038558960558809</v>
+      </c>
+      <c r="C30" s="0">
+        <v>35.114099732158877</v>
+      </c>
+      <c r="D30" s="0">
+        <v>2.8017186055174013</v>
+      </c>
+      <c r="E30" s="0">
+        <v>0.11999999999999998</v>
+      </c>
+      <c r="F30" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0">
+        <v>346</v>
+      </c>
+      <c r="B31" s="0">
+        <v>39.030456513603106</v>
+      </c>
+      <c r="C31" s="0">
+        <v>39.11521443121589</v>
+      </c>
+      <c r="D31" s="0">
+        <v>2.8230509495216856</v>
+      </c>
+      <c r="E31" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F31" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0">
+        <v>324</v>
+      </c>
+      <c r="B32" s="0">
+        <v>36.406160922878364</v>
+      </c>
+      <c r="C32" s="0">
+        <v>36.496575181789311</v>
+      </c>
+      <c r="D32" s="0">
+        <v>2.8125022337111707</v>
+      </c>
+      <c r="E32" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F32" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0">
+        <v>312</v>
+      </c>
+      <c r="B33" s="0">
+        <v>34.912000114313003</v>
+      </c>
+      <c r="C33" s="0">
+        <v>34.985711369071801</v>
+      </c>
+      <c r="D33" s="0">
+        <v>2.8005309983568001</v>
+      </c>
+      <c r="E33" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F33" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0">
+        <v>333</v>
+      </c>
+      <c r="B34" s="0">
+        <v>37.496203130873489</v>
+      </c>
+      <c r="C34" s="0">
+        <v>37.589892258425003</v>
+      </c>
+      <c r="D34" s="0">
+        <v>2.8183637519920945</v>
+      </c>
+      <c r="E34" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F34" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>321</v>
+      </c>
+      <c r="B35" s="0">
+        <v>36.037810617376984</v>
+      </c>
+      <c r="C35" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D35" s="0">
+        <v>2.8098681650359376</v>
+      </c>
+      <c r="E35" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F35" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0">
+        <v>324</v>
+      </c>
+      <c r="B36" s="0">
+        <v>36.406160922878364</v>
+      </c>
+      <c r="C36" s="0">
+        <v>36.496575181789311</v>
+      </c>
+      <c r="D36" s="0">
+        <v>2.8125022337111707</v>
+      </c>
+      <c r="E36" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F36" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0">
+        <v>321</v>
+      </c>
+      <c r="B37" s="0">
+        <v>36.037810617376984</v>
+      </c>
+      <c r="C37" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D37" s="0">
+        <v>2.8098681650359376</v>
+      </c>
+      <c r="E37" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F37" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0">
+        <v>354</v>
+      </c>
+      <c r="B38" s="0">
+        <v>39.951436974065551</v>
+      </c>
+      <c r="C38" s="0">
+        <v>40.024992192379003</v>
+      </c>
+      <c r="D38" s="0">
+        <v>2.8241550338051082</v>
+      </c>
+      <c r="E38" s="0">
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F38" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0">
+        <v>320</v>
+      </c>
+      <c r="B39" s="0">
+        <v>35.914142727222959</v>
+      </c>
+      <c r="C39" s="0">
+        <v>36</v>
+      </c>
+      <c r="D39" s="0">
+        <v>2.80897636424096</v>
+      </c>
+      <c r="E39" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F39" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0">
+        <v>333</v>
+      </c>
+      <c r="B40" s="0">
+        <v>37.496203130873489</v>
+      </c>
+      <c r="C40" s="0">
+        <v>37.589892258425003</v>
+      </c>
+      <c r="D40" s="0">
+        <v>2.8183637519920945</v>
+      </c>
+      <c r="E40" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F40" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0">
+        <v>329</v>
+      </c>
+      <c r="B41" s="0">
+        <v>37.014741709153405</v>
+      </c>
+      <c r="C41" s="0">
+        <v>37.107950630558946</v>
+      </c>
+      <c r="D41" s="0">
+        <v>2.8160384531148899</v>
+      </c>
+      <c r="E41" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F41" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0">
+        <v>321</v>
+      </c>
+      <c r="B42" s="0">
+        <v>36.037810617376984</v>
+      </c>
+      <c r="C42" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D42" s="0">
+        <v>2.8098681650359376</v>
+      </c>
+      <c r="E42" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F42" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
+        <v>321</v>
+      </c>
+      <c r="B43" s="0">
+        <v>36.037810617376984</v>
+      </c>
+      <c r="C43" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D43" s="0">
+        <v>2.8098681650359376</v>
+      </c>
+      <c r="E43" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F43" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>296</v>
+      </c>
+      <c r="B44" s="0">
+        <v>33.045788971328889</v>
+      </c>
+      <c r="C44" s="0">
+        <v>33.136083051561783</v>
+      </c>
+      <c r="D44" s="0">
+        <v>2.7947328730552767</v>
+      </c>
+      <c r="E44" s="0">
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F44" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
+        <v>300</v>
+      </c>
+      <c r="B45" s="0">
+        <v>33.468324010364114</v>
+      </c>
+      <c r="C45" s="0">
+        <v>33.541019662496844</v>
+      </c>
+      <c r="D45" s="0">
+        <v>2.7922304247514802</v>
+      </c>
+      <c r="E45" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F45" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0">
+        <v>321</v>
+      </c>
+      <c r="B46" s="0">
+        <v>36.037810617376984</v>
+      </c>
+      <c r="C46" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D46" s="0">
+        <v>2.8098681650359376</v>
+      </c>
+      <c r="E46" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F46" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0">
+        <v>321</v>
+      </c>
+      <c r="B47" s="0">
+        <v>36.037810617376984</v>
+      </c>
+      <c r="C47" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D47" s="0">
+        <v>2.8098681650359376</v>
+      </c>
+      <c r="E47" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F47" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0">
+        <v>346</v>
+      </c>
+      <c r="B48" s="0">
+        <v>39.030456513603106</v>
+      </c>
+      <c r="C48" s="0">
+        <v>39.11521443121589</v>
+      </c>
+      <c r="D48" s="0">
+        <v>2.8230509495216856</v>
+      </c>
+      <c r="E48" s="0">
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F48" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0">
+        <v>324</v>
+      </c>
+      <c r="B49" s="0">
+        <v>36.406160922878364</v>
+      </c>
+      <c r="C49" s="0">
+        <v>36.496575181789311</v>
+      </c>
+      <c r="D49" s="0">
+        <v>2.8125022337111707</v>
+      </c>
+      <c r="E49" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F49" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0">
+        <v>324</v>
+      </c>
+      <c r="B50" s="0">
+        <v>36.406160922878364</v>
+      </c>
+      <c r="C50" s="0">
+        <v>36.496575181789311</v>
+      </c>
+      <c r="D50" s="0">
+        <v>2.8125022337111707</v>
+      </c>
+      <c r="E50" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F50" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0">
+        <v>300</v>
+      </c>
+      <c r="B51" s="0">
+        <v>33.468324010364114</v>
+      </c>
+      <c r="C51" s="0">
+        <v>33.541019662496844</v>
+      </c>
+      <c r="D51" s="0">
+        <v>2.7922304247514802</v>
+      </c>
+      <c r="E51" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F51" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0">
+        <v>336</v>
+      </c>
+      <c r="B52" s="0">
+        <v>37.854275825321153</v>
+      </c>
+      <c r="C52" s="0">
+        <v>37.947331922020552</v>
+      </c>
+      <c r="D52" s="0">
+        <v>2.8198344780763467</v>
+      </c>
+      <c r="E52" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F52" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0">
+        <v>340</v>
+      </c>
+      <c r="B53" s="0">
+        <v>38.327800470486821</v>
+      </c>
+      <c r="C53" s="0">
+        <v>38.418745424597091</v>
+      </c>
+      <c r="D53" s="0">
+        <v>2.82145262403079</v>
+      </c>
+      <c r="E53" s="0">
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F53" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0">
+        <v>333</v>
+      </c>
+      <c r="B54" s="0">
+        <v>37.496203130873489</v>
+      </c>
+      <c r="C54" s="0">
+        <v>37.589892258425003</v>
+      </c>
+      <c r="D54" s="0">
+        <v>2.8183637519920945</v>
+      </c>
+      <c r="E54" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F54" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0">
+        <v>321</v>
+      </c>
+      <c r="B55" s="0">
+        <v>36.037810617376984</v>
+      </c>
+      <c r="C55" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D55" s="0">
+        <v>2.8098681650359376</v>
+      </c>
+      <c r="E55" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F55" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0">
+        <v>329</v>
+      </c>
+      <c r="B56" s="0">
+        <v>37.014741709153405</v>
+      </c>
+      <c r="C56" s="0">
+        <v>37.107950630558946</v>
+      </c>
+      <c r="D56" s="0">
+        <v>2.8160384531148899</v>
+      </c>
+      <c r="E56" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F56" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0">
+        <v>322</v>
+      </c>
+      <c r="B57" s="0">
+        <v>36.161134209563251</v>
+      </c>
+      <c r="C57" s="0">
+        <v>36.24913792078371</v>
+      </c>
+      <c r="D57" s="0">
+        <v>2.8107236898769608</v>
+      </c>
+      <c r="E57" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F57" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0">
+        <v>336</v>
+      </c>
+      <c r="B58" s="0">
+        <v>37.854275825321153</v>
+      </c>
+      <c r="C58" s="0">
+        <v>37.947331922020552</v>
+      </c>
+      <c r="D58" s="0">
+        <v>2.8198344780763467</v>
+      </c>
+      <c r="E58" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F58" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0">
+        <v>312</v>
+      </c>
+      <c r="B59" s="0">
+        <v>34.912000114313003</v>
+      </c>
+      <c r="C59" s="0">
+        <v>34.985711369071801</v>
+      </c>
+      <c r="D59" s="0">
+        <v>2.8005309983568001</v>
+      </c>
+      <c r="E59" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F59" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0">
+        <v>325</v>
+      </c>
+      <c r="B60" s="0">
+        <v>36.528496220724051</v>
+      </c>
+      <c r="C60" s="0">
+        <v>36.61966684720111</v>
+      </c>
+      <c r="D60" s="0">
+        <v>2.8132683412551933</v>
+      </c>
+      <c r="E60" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F60" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0">
+        <v>321</v>
+      </c>
+      <c r="B61" s="0">
+        <v>36.037810617376984</v>
+      </c>
+      <c r="C61" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D61" s="0">
+        <v>2.8098681650359376</v>
+      </c>
+      <c r="E61" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F61" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0">
+        <v>336</v>
+      </c>
+      <c r="B62" s="0">
+        <v>37.854275825321153</v>
+      </c>
+      <c r="C62" s="0">
+        <v>37.947331922020552</v>
+      </c>
+      <c r="D62" s="0">
+        <v>2.8198344780763467</v>
+      </c>
+      <c r="E62" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F62" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0">
+        <v>321</v>
+      </c>
+      <c r="B63" s="0">
+        <v>36.037810617376984</v>
+      </c>
+      <c r="C63" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D63" s="0">
+        <v>2.8098681650359376</v>
+      </c>
+      <c r="E63" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F63" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0">
+        <v>381</v>
+      </c>
       <c r="B64" s="0">
-        <v>0</v>
+        <v>41.585151273501786</v>
       </c>
       <c r="C64" s="0">
-        <v>0</v>
+        <v>36.496575181789311</v>
       </c>
       <c r="D64" s="0">
-        <v>0</v>
+        <v>2.7290409088465006</v>
       </c>
       <c r="E64" s="0">
         <v>0</v>
       </c>
       <c r="F64" s="0">
-        <v>0</v>
+        <v>3.0000000000000004</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0">
-        <v>0</v>
+        <v>312</v>
       </c>
       <c r="B65" s="0">
-        <v>0</v>
+        <v>34.912000114313003</v>
       </c>
       <c r="C65" s="0">
-        <v>0</v>
+        <v>34.985711369071801</v>
       </c>
       <c r="D65" s="0">
-        <v>0</v>
+        <v>2.8005309983568001</v>
       </c>
       <c r="E65" s="0">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F65" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="B66" s="0">
-        <v>0</v>
+        <v>35.914142727222959</v>
       </c>
       <c r="C66" s="0">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D66" s="0">
-        <v>0</v>
+        <v>2.80897636424096</v>
       </c>
       <c r="E66" s="0">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F66" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0">
-        <v>0</v>
+        <v>312</v>
       </c>
       <c r="B67" s="0">
-        <v>0</v>
+        <v>34.912000114313003</v>
       </c>
       <c r="C67" s="0">
-        <v>0</v>
+        <v>34.985711369071801</v>
       </c>
       <c r="D67" s="0">
-        <v>0</v>
+        <v>2.8005309983568001</v>
       </c>
       <c r="E67" s="0">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F67" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0">
-        <v>0</v>
+        <v>313</v>
       </c>
       <c r="B68" s="0">
-        <v>0</v>
+        <v>35.038558960558809</v>
       </c>
       <c r="C68" s="0">
-        <v>0</v>
+        <v>35.114099732158877</v>
       </c>
       <c r="D68" s="0">
-        <v>0</v>
+        <v>2.8017186055174013</v>
       </c>
       <c r="E68" s="0">
-        <v>0</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="F68" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="B69" s="0">
-        <v>0</v>
+        <v>33.468324010364114</v>
       </c>
       <c r="C69" s="0">
-        <v>0</v>
+        <v>33.541019662496851</v>
       </c>
       <c r="D69" s="0">
-        <v>0</v>
+        <v>2.7922304247514802</v>
       </c>
       <c r="E69" s="0">
-        <v>0</v>
+        <v>0.11999999999999998</v>
       </c>
       <c r="F69" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0">
-        <v>0</v>
+        <v>346</v>
       </c>
       <c r="B70" s="0">
-        <v>0</v>
+        <v>39.030456513603106</v>
       </c>
       <c r="C70" s="0">
-        <v>0</v>
+        <v>39.11521443121589</v>
       </c>
       <c r="D70" s="0">
-        <v>0</v>
+        <v>2.8230509495216856</v>
       </c>
       <c r="E70" s="0">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F70" s="0">
-        <v>0</v>
+        <v>3.0000000000000004</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="B71" s="0">
-        <v>0</v>
+        <v>33.468324010364114</v>
       </c>
       <c r="C71" s="0">
-        <v>0</v>
+        <v>33.541019662496844</v>
       </c>
       <c r="D71" s="0">
-        <v>0</v>
+        <v>2.7922304247514802</v>
       </c>
       <c r="E71" s="0">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F71" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0">
-        <v>0</v>
+        <v>322</v>
       </c>
       <c r="B72" s="0">
-        <v>0</v>
+        <v>36.161134209563251</v>
       </c>
       <c r="C72" s="0">
-        <v>0</v>
+        <v>36.24913792078371</v>
       </c>
       <c r="D72" s="0">
-        <v>0</v>
+        <v>2.8107236898769608</v>
       </c>
       <c r="E72" s="0">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F72" s="0">
-        <v>0</v>
+        <v>3.0000000000000004</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0">
-        <v>0</v>
+        <v>290</v>
       </c>
       <c r="B73" s="0">
-        <v>0</v>
+        <v>32.351254780494202</v>
       </c>
       <c r="C73" s="0">
-        <v>0</v>
+        <v>32.449961479175904</v>
       </c>
       <c r="D73" s="0">
-        <v>0</v>
+        <v>2.7927980299337829</v>
       </c>
       <c r="E73" s="0">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F73" s="0">
-        <v>0</v>
+        <v>3.0000000000000004</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="B74" s="0">
-        <v>0</v>
+        <v>35.914142727222959</v>
       </c>
       <c r="C74" s="0">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D74" s="0">
-        <v>0</v>
+        <v>2.80897636424096</v>
       </c>
       <c r="E74" s="0">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F74" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0">
-        <v>0</v>
+        <v>305</v>
       </c>
       <c r="B75" s="0">
-        <v>0</v>
+        <v>34.118176482294771</v>
       </c>
       <c r="C75" s="0">
-        <v>0</v>
+        <v>34.205262752974136</v>
       </c>
       <c r="D75" s="0">
-        <v>0</v>
+        <v>2.7999248397026655</v>
       </c>
       <c r="E75" s="0">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F75" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0">
-        <v>0</v>
+        <v>446</v>
       </c>
       <c r="B76" s="0">
-        <v>0</v>
+        <v>49.411985230343163</v>
       </c>
       <c r="C76" s="0">
-        <v>0</v>
+        <v>40.249223594996216</v>
       </c>
       <c r="D76" s="0">
-        <v>0</v>
+        <v>2.7698597794871658</v>
       </c>
       <c r="E76" s="0">
-        <v>0</v>
+        <v>1.3877787807814457e-17</v>
       </c>
       <c r="F76" s="0">
-        <v>0</v>
+        <v>3.0000000000000009</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0">
-        <v>0</v>
+        <v>329</v>
       </c>
       <c r="B77" s="0">
-        <v>0</v>
+        <v>37.014741709153405</v>
       </c>
       <c r="C77" s="0">
-        <v>0</v>
+        <v>37.107950630558946</v>
       </c>
       <c r="D77" s="0">
-        <v>0</v>
+        <v>2.8160384531148899</v>
       </c>
       <c r="E77" s="0">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F77" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0">
-        <v>0</v>
+        <v>324</v>
       </c>
       <c r="B78" s="0">
-        <v>0</v>
+        <v>36.406160922878364</v>
       </c>
       <c r="C78" s="0">
-        <v>0</v>
+        <v>36.496575181789311</v>
       </c>
       <c r="D78" s="0">
-        <v>0</v>
+        <v>2.8125022337111707</v>
       </c>
       <c r="E78" s="0">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F78" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0">
+        <v>305</v>
+      </c>
+      <c r="B79" s="0">
+        <v>34.118176482294778</v>
+      </c>
+      <c r="C79" s="0">
+        <v>34.205262752974143</v>
+      </c>
+      <c r="D79" s="0">
+        <v>2.7999248397026664</v>
+      </c>
+      <c r="E79" s="0">
+        <v>0.11999999999999998</v>
+      </c>
+      <c r="F79" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="0">
+        <v>333</v>
+      </c>
+      <c r="B80" s="0">
+        <v>37.496203130873489</v>
+      </c>
+      <c r="C80" s="0">
+        <v>37.589892258425003</v>
+      </c>
+      <c r="D80" s="0">
+        <v>2.8183637519920945</v>
+      </c>
+      <c r="E80" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F80" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="0">
+        <v>321</v>
+      </c>
+      <c r="B81" s="0">
+        <v>36.037810617376984</v>
+      </c>
+      <c r="C81" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D81" s="0">
+        <v>2.8098681650359376</v>
+      </c>
+      <c r="E81" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F81" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="0">
+        <v>321</v>
+      </c>
+      <c r="B82" s="0">
+        <v>36.037810617376984</v>
+      </c>
+      <c r="C82" s="0">
+        <v>36.124783736376884</v>
+      </c>
+      <c r="D82" s="0">
+        <v>2.8098681650359376</v>
+      </c>
+      <c r="E82" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F82" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="0">
+        <v>305</v>
+      </c>
+      <c r="B83" s="0">
+        <v>34.118176482294771</v>
+      </c>
+      <c r="C83" s="0">
+        <v>34.205262752974136</v>
+      </c>
+      <c r="D83" s="0">
+        <v>2.7999248397026655</v>
+      </c>
+      <c r="E83" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F83" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="0">
+        <v>360</v>
+      </c>
+      <c r="B84" s="0">
+        <v>40.717526290664516</v>
+      </c>
+      <c r="C84" s="0">
+        <v>40.804411526206337</v>
+      </c>
+      <c r="D84" s="0">
+        <v>2.8304454991108989</v>
+      </c>
+      <c r="E84" s="0">
+        <v>0.11999999999999998</v>
+      </c>
+      <c r="F84" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="0">
+        <v>340</v>
+      </c>
+      <c r="B85" s="0">
+        <v>38.327800470486821</v>
+      </c>
+      <c r="C85" s="0">
+        <v>38.418745424597091</v>
+      </c>
+      <c r="D85" s="0">
+        <v>2.82145262403079</v>
+      </c>
+      <c r="E85" s="0">
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F85" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="0">
+        <v>419</v>
+      </c>
+      <c r="B86" s="0">
+        <v>46.120541722290902</v>
+      </c>
+      <c r="C86" s="0">
+        <v>36.496575181789311</v>
+      </c>
+      <c r="D86" s="0">
+        <v>2.7521661977764711</v>
+      </c>
+      <c r="E86" s="0">
         <v>0</v>
       </c>
-      <c r="B79" s="0">
-        <v>0</v>
-      </c>
-      <c r="C79" s="0">
-        <v>0</v>
-      </c>
-      <c r="D79" s="0">
-        <v>0</v>
-      </c>
-      <c r="E79" s="0">
-        <v>0</v>
-      </c>
-      <c r="F79" s="0">
-        <v>0</v>
+      <c r="F86" s="0">
+        <v>3.0000000000000009</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="0">
+        <v>325</v>
+      </c>
+      <c r="B87" s="0">
+        <v>36.528496220724051</v>
+      </c>
+      <c r="C87" s="0">
+        <v>36.61966684720111</v>
+      </c>
+      <c r="D87" s="0">
+        <v>2.8132683412551933</v>
+      </c>
+      <c r="E87" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F87" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="0">
+        <v>329</v>
+      </c>
+      <c r="B88" s="0">
+        <v>37.014741709153405</v>
+      </c>
+      <c r="C88" s="0">
+        <v>37.107950630558946</v>
+      </c>
+      <c r="D88" s="0">
+        <v>2.8160384531148899</v>
+      </c>
+      <c r="E88" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F88" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="0">
+        <v>345</v>
+      </c>
+      <c r="B89" s="0">
+        <v>38.914142727222959</v>
+      </c>
+      <c r="C89" s="0">
+        <v>39</v>
+      </c>
+      <c r="D89" s="0">
+        <v>2.8228186566872711</v>
+      </c>
+      <c r="E89" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F89" s="0">
+        <v>3.0000000000000004</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="0">
+        <v>312</v>
+      </c>
+      <c r="B90" s="0">
+        <v>34.912000114313003</v>
+      </c>
+      <c r="C90" s="0">
+        <v>34.985711369071801</v>
+      </c>
+      <c r="D90" s="0">
+        <v>2.8005309983568001</v>
+      </c>
+      <c r="E90" s="0">
+        <v>0.12</v>
+      </c>
+      <c r="F90" s="0">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>